<commit_message>
update to include EF D line
</commit_message>
<xml_diff>
--- a/papillae counting analysis.xlsx
+++ b/papillae counting analysis.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateCount="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Line</t>
   </si>
@@ -134,14 +134,40 @@
   </si>
   <si>
     <t>HARTOEC</t>
+  </si>
+  <si>
+    <t>EFOE D</t>
+  </si>
+  <si>
+    <t>HARTOE13</t>
+  </si>
+  <si>
+    <t>HARTOE17</t>
+  </si>
+  <si>
+    <t>HARTOE19</t>
+  </si>
+  <si>
+    <t>HARTOED2</t>
+  </si>
+  <si>
+    <t>HARTOED3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,8 +195,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,19 +514,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -518,7 +545,7 @@
         <v>70380</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E29" si="0">C2/(D2/10000)</f>
+        <f t="shared" ref="E2:E34" si="0">C2/(D2/10000)</f>
         <v>5.3992611537368571</v>
       </c>
       <c r="F2">
@@ -1059,7 +1086,107 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <f>372*497</f>
+        <v>184884</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.27043984336124277</v>
+      </c>
+      <c r="F30">
+        <f>AVERAGE(E30:E34)</f>
+        <v>0.23413974146449137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>306*229</f>
+        <v>70074</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <f>995*749</f>
+        <v>745255</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>4.0254677929031007E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f>384*288</f>
+        <v>110592</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>9.0422453703703692E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <f>369*493</f>
+        <v>181917</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.76958173232847948</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>